<commit_message>
Organisation + nouvelle vue à jour
</commit_message>
<xml_diff>
--- a/Création jeu de données/insert compo ordre.xlsx
+++ b/Création jeu de données/insert compo ordre.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bevilaro\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{334482AB-4AF6-47CD-9B1A-08DDD4746BED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EAB358-FC65-4F48-AC3D-4AE338254ECC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7980" xr2:uid="{AE96EF8C-B29E-4422-8A67-F5FA269D26C1}"/>
   </bookViews>
   <sheets>
     <sheet name="T_J_composition_ordre_com" sheetId="1" r:id="rId1"/>
+    <sheet name="T_J_SEMAINE_THEMATIQUE_SET" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>numero_ordre</t>
   </si>
@@ -37,6 +38,12 @@
   </si>
   <si>
     <t>quantite_objet</t>
+  </si>
+  <si>
+    <t>numero_thematique</t>
+  </si>
+  <si>
+    <t>numero_semaine</t>
   </si>
 </sst>
 </file>
@@ -391,7 +398,7 @@
   <dimension ref="A1:D140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,11 +426,11 @@
       </c>
       <c r="C2">
         <f ca="1">(RANDBETWEEN(10,50)*1000)</f>
-        <v>42000</v>
+        <v>44000</v>
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(10,40)</f>
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -435,11 +442,11 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C66" ca="1" si="0">(RANDBETWEEN(10,50)*1000)</f>
-        <v>24000</v>
+        <v>39000</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D66" ca="1" si="1">RANDBETWEEN(10,40)</f>
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -451,11 +458,11 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>49000</v>
+        <v>36000</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -467,11 +474,11 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>11000</v>
+        <v>47000</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -483,11 +490,11 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>46000</v>
+        <v>21000</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -499,7 +506,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>41000</v>
+        <v>28000</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
@@ -515,11 +522,11 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>18000</v>
+        <v>45000</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -531,11 +538,11 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>20000</v>
+        <v>26000</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -547,11 +554,11 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>41000</v>
+        <v>44000</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -563,11 +570,11 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -579,11 +586,11 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>18000</v>
+        <v>40000</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -595,11 +602,11 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>44000</v>
+        <v>23000</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -611,11 +618,11 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>26000</v>
+        <v>13000</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -627,11 +634,11 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -643,7 +650,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>33000</v>
+        <v>39000</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
@@ -659,11 +666,11 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>18000</v>
+        <v>21000</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -675,11 +682,11 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>20000</v>
+        <v>29000</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -691,11 +698,11 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>41000</v>
+        <v>38000</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -707,11 +714,11 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>22000</v>
+        <v>28000</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -723,7 +730,7 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>22000</v>
+        <v>16000</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
@@ -739,11 +746,11 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>29000</v>
+        <v>41000</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -755,11 +762,11 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>46000</v>
+        <v>41000</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -771,11 +778,11 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>40000</v>
+        <v>26000</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -787,11 +794,11 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>37000</v>
+        <v>17000</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -803,11 +810,11 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>48000</v>
+        <v>49000</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -819,11 +826,11 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>27000</v>
+        <v>11000</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -835,11 +842,11 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="0"/>
-        <v>30000</v>
+        <v>35000</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -851,11 +858,11 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="0"/>
-        <v>33000</v>
+        <v>45000</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -867,11 +874,11 @@
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="0"/>
-        <v>32000</v>
+        <v>41000</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -883,11 +890,11 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="0"/>
-        <v>25000</v>
+        <v>36000</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="1"/>
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -899,11 +906,11 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="0"/>
-        <v>38000</v>
+        <v>26000</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -915,11 +922,11 @@
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="0"/>
-        <v>47000</v>
+        <v>30000</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -931,11 +938,11 @@
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="0"/>
-        <v>34000</v>
+        <v>46000</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -947,11 +954,11 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="0"/>
-        <v>22000</v>
+        <v>46000</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -963,11 +970,11 @@
       </c>
       <c r="C36">
         <f t="shared" ca="1" si="0"/>
-        <v>18000</v>
+        <v>19000</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -979,11 +986,11 @@
       </c>
       <c r="C37">
         <f t="shared" ca="1" si="0"/>
-        <v>48000</v>
+        <v>12000</v>
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -995,11 +1002,11 @@
       </c>
       <c r="C38">
         <f t="shared" ca="1" si="0"/>
-        <v>30000</v>
+        <v>46000</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1011,11 +1018,11 @@
       </c>
       <c r="C39">
         <f t="shared" ca="1" si="0"/>
-        <v>28000</v>
+        <v>26000</v>
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1027,11 +1034,11 @@
       </c>
       <c r="C40">
         <f t="shared" ca="1" si="0"/>
-        <v>37000</v>
+        <v>49000</v>
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1043,11 +1050,11 @@
       </c>
       <c r="C41">
         <f t="shared" ca="1" si="0"/>
-        <v>50000</v>
+        <v>32000</v>
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1059,11 +1066,11 @@
       </c>
       <c r="C42">
         <f t="shared" ca="1" si="0"/>
-        <v>41000</v>
+        <v>16000</v>
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1075,11 +1082,11 @@
       </c>
       <c r="C43">
         <f t="shared" ca="1" si="0"/>
-        <v>15000</v>
+        <v>12000</v>
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1091,11 +1098,11 @@
       </c>
       <c r="C44">
         <f t="shared" ca="1" si="0"/>
-        <v>31000</v>
+        <v>50000</v>
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1107,11 +1114,11 @@
       </c>
       <c r="C45">
         <f t="shared" ca="1" si="0"/>
-        <v>47000</v>
+        <v>14000</v>
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1123,11 +1130,11 @@
       </c>
       <c r="C46">
         <f t="shared" ca="1" si="0"/>
-        <v>47000</v>
+        <v>27000</v>
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1139,11 +1146,11 @@
       </c>
       <c r="C47">
         <f t="shared" ca="1" si="0"/>
-        <v>31000</v>
+        <v>17000</v>
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1155,11 +1162,11 @@
       </c>
       <c r="C48">
         <f t="shared" ca="1" si="0"/>
-        <v>25000</v>
+        <v>32000</v>
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1171,11 +1178,11 @@
       </c>
       <c r="C49">
         <f t="shared" ca="1" si="0"/>
-        <v>41000</v>
+        <v>27000</v>
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1187,11 +1194,11 @@
       </c>
       <c r="C50">
         <f t="shared" ca="1" si="0"/>
-        <v>25000</v>
+        <v>14000</v>
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1203,11 +1210,11 @@
       </c>
       <c r="C51">
         <f t="shared" ca="1" si="0"/>
-        <v>14000</v>
+        <v>42000</v>
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1219,11 +1226,11 @@
       </c>
       <c r="C52">
         <f t="shared" ca="1" si="0"/>
-        <v>49000</v>
+        <v>16000</v>
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1235,11 +1242,11 @@
       </c>
       <c r="C53">
         <f t="shared" ca="1" si="0"/>
-        <v>39000</v>
+        <v>50000</v>
       </c>
       <c r="D53">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1251,11 +1258,11 @@
       </c>
       <c r="C54">
         <f t="shared" ca="1" si="0"/>
-        <v>32000</v>
+        <v>49000</v>
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1267,11 +1274,11 @@
       </c>
       <c r="C55">
         <f t="shared" ca="1" si="0"/>
-        <v>21000</v>
+        <v>43000</v>
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1283,11 +1290,11 @@
       </c>
       <c r="C56">
         <f t="shared" ca="1" si="0"/>
-        <v>32000</v>
+        <v>34000</v>
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1299,11 +1306,11 @@
       </c>
       <c r="C57">
         <f t="shared" ca="1" si="0"/>
-        <v>21000</v>
+        <v>32000</v>
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1315,11 +1322,11 @@
       </c>
       <c r="C58">
         <f t="shared" ca="1" si="0"/>
-        <v>27000</v>
+        <v>12000</v>
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1331,11 +1338,11 @@
       </c>
       <c r="C59">
         <f t="shared" ca="1" si="0"/>
-        <v>37000</v>
+        <v>12000</v>
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1347,11 +1354,11 @@
       </c>
       <c r="C60">
         <f t="shared" ca="1" si="0"/>
-        <v>43000</v>
+        <v>39000</v>
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1363,11 +1370,11 @@
       </c>
       <c r="C61">
         <f t="shared" ca="1" si="0"/>
-        <v>47000</v>
+        <v>26000</v>
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1379,11 +1386,11 @@
       </c>
       <c r="C62">
         <f t="shared" ca="1" si="0"/>
-        <v>32000</v>
+        <v>14000</v>
       </c>
       <c r="D62">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1395,11 +1402,11 @@
       </c>
       <c r="C63">
         <f t="shared" ca="1" si="0"/>
-        <v>10000</v>
+        <v>35000</v>
       </c>
       <c r="D63">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1411,11 +1418,11 @@
       </c>
       <c r="C64">
         <f t="shared" ca="1" si="0"/>
-        <v>21000</v>
+        <v>49000</v>
       </c>
       <c r="D64">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1427,11 +1434,11 @@
       </c>
       <c r="C65">
         <f t="shared" ca="1" si="0"/>
-        <v>19000</v>
+        <v>47000</v>
       </c>
       <c r="D65">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1443,11 +1450,11 @@
       </c>
       <c r="C66">
         <f t="shared" ca="1" si="0"/>
-        <v>11000</v>
+        <v>45000</v>
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1459,11 +1466,11 @@
       </c>
       <c r="C67">
         <f t="shared" ref="C67:C130" ca="1" si="2">(RANDBETWEEN(10,50)*1000)</f>
-        <v>46000</v>
+        <v>31000</v>
       </c>
       <c r="D67">
         <f t="shared" ref="D67:D130" ca="1" si="3">RANDBETWEEN(10,40)</f>
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1475,7 +1482,7 @@
       </c>
       <c r="C68">
         <f t="shared" ca="1" si="2"/>
-        <v>41000</v>
+        <v>27000</v>
       </c>
       <c r="D68">
         <f t="shared" ca="1" si="3"/>
@@ -1491,11 +1498,11 @@
       </c>
       <c r="C69">
         <f t="shared" ca="1" si="2"/>
-        <v>11000</v>
+        <v>38000</v>
       </c>
       <c r="D69">
         <f t="shared" ca="1" si="3"/>
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1507,11 +1514,11 @@
       </c>
       <c r="C70">
         <f t="shared" ca="1" si="2"/>
-        <v>43000</v>
+        <v>26000</v>
       </c>
       <c r="D70">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1523,11 +1530,11 @@
       </c>
       <c r="C71">
         <f t="shared" ca="1" si="2"/>
-        <v>22000</v>
+        <v>35000</v>
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="3"/>
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1539,11 +1546,11 @@
       </c>
       <c r="C72">
         <f t="shared" ca="1" si="2"/>
-        <v>26000</v>
+        <v>41000</v>
       </c>
       <c r="D72">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1555,11 +1562,11 @@
       </c>
       <c r="C73">
         <f t="shared" ca="1" si="2"/>
-        <v>50000</v>
+        <v>35000</v>
       </c>
       <c r="D73">
         <f t="shared" ca="1" si="3"/>
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1571,11 +1578,11 @@
       </c>
       <c r="C74">
         <f t="shared" ca="1" si="2"/>
-        <v>20000</v>
+        <v>42000</v>
       </c>
       <c r="D74">
         <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1587,11 +1594,11 @@
       </c>
       <c r="C75">
         <f t="shared" ca="1" si="2"/>
-        <v>24000</v>
+        <v>42000</v>
       </c>
       <c r="D75">
         <f t="shared" ca="1" si="3"/>
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1603,11 +1610,11 @@
       </c>
       <c r="C76">
         <f t="shared" ca="1" si="2"/>
-        <v>15000</v>
+        <v>28000</v>
       </c>
       <c r="D76">
         <f t="shared" ca="1" si="3"/>
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1619,11 +1626,11 @@
       </c>
       <c r="C77">
         <f t="shared" ca="1" si="2"/>
-        <v>44000</v>
+        <v>15000</v>
       </c>
       <c r="D77">
         <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1635,11 +1642,11 @@
       </c>
       <c r="C78">
         <f t="shared" ca="1" si="2"/>
-        <v>27000</v>
+        <v>41000</v>
       </c>
       <c r="D78">
         <f t="shared" ca="1" si="3"/>
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1651,11 +1658,11 @@
       </c>
       <c r="C79">
         <f t="shared" ca="1" si="2"/>
-        <v>49000</v>
+        <v>16000</v>
       </c>
       <c r="D79">
         <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1667,11 +1674,11 @@
       </c>
       <c r="C80">
         <f t="shared" ca="1" si="2"/>
-        <v>12000</v>
+        <v>13000</v>
       </c>
       <c r="D80">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1683,11 +1690,11 @@
       </c>
       <c r="C81">
         <f t="shared" ca="1" si="2"/>
-        <v>31000</v>
+        <v>24000</v>
       </c>
       <c r="D81">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1699,11 +1706,11 @@
       </c>
       <c r="C82">
         <f t="shared" ca="1" si="2"/>
-        <v>35000</v>
+        <v>49000</v>
       </c>
       <c r="D82">
         <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1715,11 +1722,11 @@
       </c>
       <c r="C83">
         <f t="shared" ca="1" si="2"/>
-        <v>29000</v>
+        <v>12000</v>
       </c>
       <c r="D83">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1731,11 +1738,11 @@
       </c>
       <c r="C84">
         <f t="shared" ca="1" si="2"/>
-        <v>47000</v>
+        <v>17000</v>
       </c>
       <c r="D84">
         <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <v>37</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1747,11 +1754,11 @@
       </c>
       <c r="C85">
         <f t="shared" ca="1" si="2"/>
-        <v>37000</v>
+        <v>19000</v>
       </c>
       <c r="D85">
         <f t="shared" ca="1" si="3"/>
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1763,11 +1770,11 @@
       </c>
       <c r="C86">
         <f t="shared" ca="1" si="2"/>
-        <v>22000</v>
+        <v>38000</v>
       </c>
       <c r="D86">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1779,11 +1786,11 @@
       </c>
       <c r="C87">
         <f t="shared" ca="1" si="2"/>
-        <v>15000</v>
+        <v>11000</v>
       </c>
       <c r="D87">
         <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1795,11 +1802,11 @@
       </c>
       <c r="C88">
         <f t="shared" ca="1" si="2"/>
-        <v>20000</v>
+        <v>41000</v>
       </c>
       <c r="D88">
         <f t="shared" ca="1" si="3"/>
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1815,7 +1822,7 @@
       </c>
       <c r="D89">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1827,11 +1834,11 @@
       </c>
       <c r="C90">
         <f t="shared" ca="1" si="2"/>
-        <v>45000</v>
+        <v>46000</v>
       </c>
       <c r="D90">
         <f t="shared" ca="1" si="3"/>
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -1843,11 +1850,11 @@
       </c>
       <c r="C91">
         <f t="shared" ca="1" si="2"/>
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="D91">
         <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -1859,11 +1866,11 @@
       </c>
       <c r="C92">
         <f t="shared" ca="1" si="2"/>
-        <v>23000</v>
+        <v>43000</v>
       </c>
       <c r="D92">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1875,11 +1882,11 @@
       </c>
       <c r="C93">
         <f t="shared" ca="1" si="2"/>
-        <v>27000</v>
+        <v>48000</v>
       </c>
       <c r="D93">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -1891,11 +1898,11 @@
       </c>
       <c r="C94">
         <f t="shared" ca="1" si="2"/>
-        <v>12000</v>
+        <v>25000</v>
       </c>
       <c r="D94">
         <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -1907,11 +1914,11 @@
       </c>
       <c r="C95">
         <f t="shared" ca="1" si="2"/>
-        <v>37000</v>
+        <v>19000</v>
       </c>
       <c r="D95">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -1923,11 +1930,11 @@
       </c>
       <c r="C96">
         <f t="shared" ca="1" si="2"/>
-        <v>38000</v>
+        <v>24000</v>
       </c>
       <c r="D96">
         <f t="shared" ca="1" si="3"/>
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -1939,11 +1946,11 @@
       </c>
       <c r="C97">
         <f t="shared" ca="1" si="2"/>
-        <v>24000</v>
+        <v>17000</v>
       </c>
       <c r="D97">
         <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1959,7 +1966,7 @@
       </c>
       <c r="D98">
         <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1971,11 +1978,11 @@
       </c>
       <c r="C99">
         <f t="shared" ca="1" si="2"/>
-        <v>25000</v>
+        <v>50000</v>
       </c>
       <c r="D99">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -1987,11 +1994,11 @@
       </c>
       <c r="C100">
         <f t="shared" ca="1" si="2"/>
-        <v>39000</v>
+        <v>11000</v>
       </c>
       <c r="D100">
         <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2003,11 +2010,11 @@
       </c>
       <c r="C101">
         <f t="shared" ca="1" si="2"/>
-        <v>32000</v>
+        <v>41000</v>
       </c>
       <c r="D101">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2019,11 +2026,11 @@
       </c>
       <c r="C102">
         <f t="shared" ca="1" si="2"/>
-        <v>12000</v>
+        <v>48000</v>
       </c>
       <c r="D102">
         <f t="shared" ca="1" si="3"/>
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2035,11 +2042,11 @@
       </c>
       <c r="C103">
         <f t="shared" ca="1" si="2"/>
-        <v>42000</v>
+        <v>46000</v>
       </c>
       <c r="D103">
         <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2051,11 +2058,11 @@
       </c>
       <c r="C104">
         <f t="shared" ca="1" si="2"/>
-        <v>18000</v>
+        <v>19000</v>
       </c>
       <c r="D104">
         <f t="shared" ca="1" si="3"/>
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2067,11 +2074,11 @@
       </c>
       <c r="C105">
         <f t="shared" ca="1" si="2"/>
-        <v>11000</v>
+        <v>49000</v>
       </c>
       <c r="D105">
         <f t="shared" ca="1" si="3"/>
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2083,11 +2090,11 @@
       </c>
       <c r="C106">
         <f t="shared" ca="1" si="2"/>
-        <v>20000</v>
+        <v>23000</v>
       </c>
       <c r="D106">
         <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2099,11 +2106,11 @@
       </c>
       <c r="C107">
         <f t="shared" ca="1" si="2"/>
-        <v>39000</v>
+        <v>14000</v>
       </c>
       <c r="D107">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2115,11 +2122,11 @@
       </c>
       <c r="C108">
         <f t="shared" ca="1" si="2"/>
-        <v>28000</v>
+        <v>39000</v>
       </c>
       <c r="D108">
         <f t="shared" ca="1" si="3"/>
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2131,11 +2138,11 @@
       </c>
       <c r="C109">
         <f t="shared" ca="1" si="2"/>
-        <v>21000</v>
+        <v>45000</v>
       </c>
       <c r="D109">
         <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2147,11 +2154,11 @@
       </c>
       <c r="C110">
         <f t="shared" ca="1" si="2"/>
-        <v>40000</v>
+        <v>18000</v>
       </c>
       <c r="D110">
         <f t="shared" ca="1" si="3"/>
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2163,11 +2170,11 @@
       </c>
       <c r="C111">
         <f t="shared" ca="1" si="2"/>
-        <v>50000</v>
+        <v>31000</v>
       </c>
       <c r="D111">
         <f t="shared" ca="1" si="3"/>
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2179,11 +2186,11 @@
       </c>
       <c r="C112">
         <f t="shared" ca="1" si="2"/>
-        <v>33000</v>
+        <v>20000</v>
       </c>
       <c r="D112">
         <f t="shared" ca="1" si="3"/>
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2195,11 +2202,11 @@
       </c>
       <c r="C113">
         <f t="shared" ca="1" si="2"/>
-        <v>16000</v>
+        <v>37000</v>
       </c>
       <c r="D113">
         <f t="shared" ca="1" si="3"/>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2211,7 +2218,7 @@
       </c>
       <c r="C114">
         <f t="shared" ca="1" si="2"/>
-        <v>16000</v>
+        <v>50000</v>
       </c>
       <c r="D114">
         <f t="shared" ca="1" si="3"/>
@@ -2227,11 +2234,11 @@
       </c>
       <c r="C115">
         <f t="shared" ca="1" si="2"/>
-        <v>42000</v>
+        <v>50000</v>
       </c>
       <c r="D115">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2243,11 +2250,11 @@
       </c>
       <c r="C116">
         <f t="shared" ca="1" si="2"/>
-        <v>29000</v>
+        <v>16000</v>
       </c>
       <c r="D116">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,11 +2266,11 @@
       </c>
       <c r="C117">
         <f t="shared" ca="1" si="2"/>
-        <v>35000</v>
+        <v>12000</v>
       </c>
       <c r="D117">
         <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2275,11 +2282,11 @@
       </c>
       <c r="C118">
         <f t="shared" ca="1" si="2"/>
-        <v>48000</v>
+        <v>22000</v>
       </c>
       <c r="D118">
         <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2291,11 +2298,11 @@
       </c>
       <c r="C119">
         <f t="shared" ca="1" si="2"/>
-        <v>42000</v>
+        <v>30000</v>
       </c>
       <c r="D119">
         <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2307,11 +2314,11 @@
       </c>
       <c r="C120">
         <f t="shared" ca="1" si="2"/>
-        <v>23000</v>
+        <v>21000</v>
       </c>
       <c r="D120">
         <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2323,11 +2330,11 @@
       </c>
       <c r="C121">
         <f t="shared" ca="1" si="2"/>
-        <v>39000</v>
+        <v>30000</v>
       </c>
       <c r="D121">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2339,11 +2346,11 @@
       </c>
       <c r="C122">
         <f t="shared" ca="1" si="2"/>
-        <v>12000</v>
+        <v>14000</v>
       </c>
       <c r="D122">
         <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2355,11 +2362,11 @@
       </c>
       <c r="C123">
         <f t="shared" ca="1" si="2"/>
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="D123">
         <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2371,11 +2378,11 @@
       </c>
       <c r="C124">
         <f t="shared" ca="1" si="2"/>
-        <v>15000</v>
+        <v>34000</v>
       </c>
       <c r="D124">
         <f t="shared" ca="1" si="3"/>
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2387,11 +2394,11 @@
       </c>
       <c r="C125">
         <f t="shared" ca="1" si="2"/>
-        <v>40000</v>
+        <v>34000</v>
       </c>
       <c r="D125">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -2403,11 +2410,11 @@
       </c>
       <c r="C126">
         <f t="shared" ca="1" si="2"/>
-        <v>26000</v>
+        <v>41000</v>
       </c>
       <c r="D126">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2419,11 +2426,11 @@
       </c>
       <c r="C127">
         <f t="shared" ca="1" si="2"/>
-        <v>17000</v>
+        <v>25000</v>
       </c>
       <c r="D127">
         <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -2435,11 +2442,11 @@
       </c>
       <c r="C128">
         <f t="shared" ca="1" si="2"/>
-        <v>10000</v>
+        <v>34000</v>
       </c>
       <c r="D128">
         <f t="shared" ca="1" si="3"/>
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -2451,11 +2458,11 @@
       </c>
       <c r="C129">
         <f t="shared" ca="1" si="2"/>
-        <v>33000</v>
+        <v>26000</v>
       </c>
       <c r="D129">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -2467,7 +2474,7 @@
       </c>
       <c r="C130">
         <f t="shared" ca="1" si="2"/>
-        <v>30000</v>
+        <v>33000</v>
       </c>
       <c r="D130">
         <f t="shared" ca="1" si="3"/>
@@ -2483,11 +2490,11 @@
       </c>
       <c r="C131">
         <f t="shared" ref="C131:C148" ca="1" si="4">(RANDBETWEEN(10,50)*1000)</f>
-        <v>46000</v>
+        <v>35000</v>
       </c>
       <c r="D131">
         <f t="shared" ref="D131:D148" ca="1" si="5">RANDBETWEEN(10,40)</f>
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2499,11 +2506,11 @@
       </c>
       <c r="C132">
         <f t="shared" ca="1" si="4"/>
-        <v>44000</v>
+        <v>23000</v>
       </c>
       <c r="D132">
         <f t="shared" ca="1" si="5"/>
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -2515,11 +2522,11 @@
       </c>
       <c r="C133">
         <f t="shared" ca="1" si="4"/>
-        <v>32000</v>
+        <v>37000</v>
       </c>
       <c r="D133">
         <f t="shared" ca="1" si="5"/>
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -2531,11 +2538,11 @@
       </c>
       <c r="C134">
         <f t="shared" ca="1" si="4"/>
-        <v>50000</v>
+        <v>20000</v>
       </c>
       <c r="D134">
         <f t="shared" ca="1" si="5"/>
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -2547,11 +2554,11 @@
       </c>
       <c r="C135">
         <f t="shared" ca="1" si="4"/>
-        <v>23000</v>
+        <v>10000</v>
       </c>
       <c r="D135">
         <f t="shared" ca="1" si="5"/>
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -2563,7 +2570,7 @@
       </c>
       <c r="C136">
         <f t="shared" ca="1" si="4"/>
-        <v>37000</v>
+        <v>40000</v>
       </c>
       <c r="D136">
         <f t="shared" ca="1" si="5"/>
@@ -2579,11 +2586,11 @@
       </c>
       <c r="C137">
         <f t="shared" ca="1" si="4"/>
-        <v>25000</v>
+        <v>39000</v>
       </c>
       <c r="D137">
         <f t="shared" ca="1" si="5"/>
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -2595,11 +2602,11 @@
       </c>
       <c r="C138">
         <f t="shared" ca="1" si="4"/>
-        <v>14000</v>
+        <v>30000</v>
       </c>
       <c r="D138">
         <f t="shared" ca="1" si="5"/>
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -2611,11 +2618,11 @@
       </c>
       <c r="C139">
         <f t="shared" ca="1" si="4"/>
-        <v>47000</v>
+        <v>21000</v>
       </c>
       <c r="D139">
         <f t="shared" ca="1" si="5"/>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -2627,11 +2634,1578 @@
       </c>
       <c r="C140">
         <f t="shared" ca="1" si="4"/>
-        <v>28000</v>
+        <v>23000</v>
       </c>
       <c r="D140">
         <f t="shared" ca="1" si="5"/>
-        <v>35</v>
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF094594-BE27-4B31-89D1-70AD7773E6C9}">
+  <dimension ref="A1:B194"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>8</v>
+      </c>
+      <c r="B36">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>14</v>
+      </c>
+      <c r="B39">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>8</v>
+      </c>
+      <c r="B40">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>4</v>
+      </c>
+      <c r="B51">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>6</v>
+      </c>
+      <c r="B52">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>14</v>
+      </c>
+      <c r="B54">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>9</v>
+      </c>
+      <c r="B55">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>6</v>
+      </c>
+      <c r="B56">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2</v>
+      </c>
+      <c r="B57">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>15</v>
+      </c>
+      <c r="B59">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>11</v>
+      </c>
+      <c r="B61">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2</v>
+      </c>
+      <c r="B62">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>10</v>
+      </c>
+      <c r="B64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>12</v>
+      </c>
+      <c r="B65">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>11</v>
+      </c>
+      <c r="B66">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>4</v>
+      </c>
+      <c r="B67">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>13</v>
+      </c>
+      <c r="B68">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2</v>
+      </c>
+      <c r="B70">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>15</v>
+      </c>
+      <c r="B71">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2</v>
+      </c>
+      <c r="B72">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>10</v>
+      </c>
+      <c r="B73">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>11</v>
+      </c>
+      <c r="B74">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>13</v>
+      </c>
+      <c r="B75">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>1</v>
+      </c>
+      <c r="B76">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>11</v>
+      </c>
+      <c r="B77">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>5</v>
+      </c>
+      <c r="B78">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>12</v>
+      </c>
+      <c r="B79">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>13</v>
+      </c>
+      <c r="B80">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>15</v>
+      </c>
+      <c r="B81">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>7</v>
+      </c>
+      <c r="B82">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>9</v>
+      </c>
+      <c r="B83">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>11</v>
+      </c>
+      <c r="B84">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>12</v>
+      </c>
+      <c r="B85">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>5</v>
+      </c>
+      <c r="B86">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>4</v>
+      </c>
+      <c r="B87">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>9</v>
+      </c>
+      <c r="B88">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>14</v>
+      </c>
+      <c r="B89">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>5</v>
+      </c>
+      <c r="B90">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>5</v>
+      </c>
+      <c r="B91">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>13</v>
+      </c>
+      <c r="B92">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>11</v>
+      </c>
+      <c r="B93">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>5</v>
+      </c>
+      <c r="B94">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>4</v>
+      </c>
+      <c r="B95">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>10</v>
+      </c>
+      <c r="B96">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>9</v>
+      </c>
+      <c r="B97">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>2</v>
+      </c>
+      <c r="B98">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>8</v>
+      </c>
+      <c r="B99">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>1</v>
+      </c>
+      <c r="B100">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>9</v>
+      </c>
+      <c r="B101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>2</v>
+      </c>
+      <c r="B102">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>8</v>
+      </c>
+      <c r="B103">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>14</v>
+      </c>
+      <c r="B104">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>6</v>
+      </c>
+      <c r="B105">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>2</v>
+      </c>
+      <c r="B106">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>3</v>
+      </c>
+      <c r="B107">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>7</v>
+      </c>
+      <c r="B108">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>5</v>
+      </c>
+      <c r="B109">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>6</v>
+      </c>
+      <c r="B110">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>6</v>
+      </c>
+      <c r="B111">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>2</v>
+      </c>
+      <c r="B112">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>3</v>
+      </c>
+      <c r="B113">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>15</v>
+      </c>
+      <c r="B114">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>7</v>
+      </c>
+      <c r="B115">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>1</v>
+      </c>
+      <c r="B116">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>5</v>
+      </c>
+      <c r="B117">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>9</v>
+      </c>
+      <c r="B118">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>15</v>
+      </c>
+      <c r="B119">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>14</v>
+      </c>
+      <c r="B120">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>14</v>
+      </c>
+      <c r="B121">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>3</v>
+      </c>
+      <c r="B122">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>9</v>
+      </c>
+      <c r="B123">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>1</v>
+      </c>
+      <c r="B124">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>12</v>
+      </c>
+      <c r="B125">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>8</v>
+      </c>
+      <c r="B126">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>9</v>
+      </c>
+      <c r="B127">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>4</v>
+      </c>
+      <c r="B128">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>10</v>
+      </c>
+      <c r="B129">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>12</v>
+      </c>
+      <c r="B130">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>15</v>
+      </c>
+      <c r="B131">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>15</v>
+      </c>
+      <c r="B132">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>4</v>
+      </c>
+      <c r="B133">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>3</v>
+      </c>
+      <c r="B134">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>1</v>
+      </c>
+      <c r="B135">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>11</v>
+      </c>
+      <c r="B136">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>8</v>
+      </c>
+      <c r="B137">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>9</v>
+      </c>
+      <c r="B138">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>3</v>
+      </c>
+      <c r="B139">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>8</v>
+      </c>
+      <c r="B140">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>2</v>
+      </c>
+      <c r="B141">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>15</v>
+      </c>
+      <c r="B142">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>7</v>
+      </c>
+      <c r="B143">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>15</v>
+      </c>
+      <c r="B144">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>8</v>
+      </c>
+      <c r="B145">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>3</v>
+      </c>
+      <c r="B146">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>4</v>
+      </c>
+      <c r="B147">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>2</v>
+      </c>
+      <c r="B148">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>10</v>
+      </c>
+      <c r="B149">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>9</v>
+      </c>
+      <c r="B150">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>10</v>
+      </c>
+      <c r="B151">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>8</v>
+      </c>
+      <c r="B152">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>10</v>
+      </c>
+      <c r="B153">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>14</v>
+      </c>
+      <c r="B154">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>1</v>
+      </c>
+      <c r="B155">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>4</v>
+      </c>
+      <c r="B156">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>7</v>
+      </c>
+      <c r="B157">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>3</v>
+      </c>
+      <c r="B158">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>6</v>
+      </c>
+      <c r="B159">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>6</v>
+      </c>
+      <c r="B160">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>11</v>
+      </c>
+      <c r="B161">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>6</v>
+      </c>
+      <c r="B162">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>3</v>
+      </c>
+      <c r="B163">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>5</v>
+      </c>
+      <c r="B164">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>5</v>
+      </c>
+      <c r="B165">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>12</v>
+      </c>
+      <c r="B166">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>2</v>
+      </c>
+      <c r="B167">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>11</v>
+      </c>
+      <c r="B168">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>12</v>
+      </c>
+      <c r="B169">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>15</v>
+      </c>
+      <c r="B170">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>6</v>
+      </c>
+      <c r="B171">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>6</v>
+      </c>
+      <c r="B172">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>4</v>
+      </c>
+      <c r="B173">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>2</v>
+      </c>
+      <c r="B174">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>13</v>
+      </c>
+      <c r="B175">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>14</v>
+      </c>
+      <c r="B176">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>6</v>
+      </c>
+      <c r="B177">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>5</v>
+      </c>
+      <c r="B178">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>13</v>
+      </c>
+      <c r="B179">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>10</v>
+      </c>
+      <c r="B180">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>9</v>
+      </c>
+      <c r="B181">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>5</v>
+      </c>
+      <c r="B182">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>3</v>
+      </c>
+      <c r="B183">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>8</v>
+      </c>
+      <c r="B184">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>10</v>
+      </c>
+      <c r="B185">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>11</v>
+      </c>
+      <c r="B186">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>8</v>
+      </c>
+      <c r="B187">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>1</v>
+      </c>
+      <c r="B188">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>10</v>
+      </c>
+      <c r="B189">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>5</v>
+      </c>
+      <c r="B190">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>9</v>
+      </c>
+      <c r="B191">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>6</v>
+      </c>
+      <c r="B192">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>14</v>
+      </c>
+      <c r="B193">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>9</v>
+      </c>
+      <c r="B194">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>